<commit_message>
reset prey mass to 1; added single ind plot
</commit_message>
<xml_diff>
--- a/CA Otter Tissues.xlsx
+++ b/CA Otter Tissues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="0" windowWidth="25040" windowHeight="15500"/>
+    <workbookView xWindow="1300" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1819" uniqueCount="548">
   <si>
     <t>SO 7112-14</t>
   </si>
@@ -1676,6 +1676,9 @@
   </si>
   <si>
     <t>tissue.type</t>
+  </si>
+  <si>
+    <t>Range</t>
   </si>
 </sst>
 </file>
@@ -1777,10 +1780,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="979">
+  <cellStyleXfs count="1013">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2889,7 +2926,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="979">
+  <cellStyles count="1013">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3379,6 +3416,23 @@
     <cellStyle name="Followed Hyperlink" xfId="974" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="976" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="996" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="998" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1000" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1002" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1004" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1006" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1008" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1012" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -3867,6 +3921,23 @@
     <cellStyle name="Hyperlink" xfId="973" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="975" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="995" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="997" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="999" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1001" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1003" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1005" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1007" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1009" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1011" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
@@ -4021,11 +4092,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2140499864"/>
-        <c:axId val="2141052680"/>
+        <c:axId val="-2088135752"/>
+        <c:axId val="-2084702376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2140499864"/>
+        <c:axId val="-2088135752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4034,7 +4105,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141052680"/>
+        <c:crossAx val="-2084702376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4042,7 +4113,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141052680"/>
+        <c:axId val="-2084702376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="12.0"/>
@@ -4054,7 +4125,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140499864"/>
+        <c:crossAx val="-2088135752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4188,11 +4259,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2140943608"/>
-        <c:axId val="2140900696"/>
+        <c:axId val="-2084122312"/>
+        <c:axId val="-2083766264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2140943608"/>
+        <c:axId val="-2084122312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4201,7 +4272,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140900696"/>
+        <c:crossAx val="-2083766264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4209,7 +4280,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2140900696"/>
+        <c:axId val="-2083766264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -4221,7 +4292,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2140943608"/>
+        <c:crossAx val="-2084122312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4488,11 +4559,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2141144664"/>
-        <c:axId val="2141147576"/>
+        <c:axId val="-2085273656"/>
+        <c:axId val="-2107694440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2141144664"/>
+        <c:axId val="-2085273656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4501,7 +4572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141147576"/>
+        <c:crossAx val="-2107694440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4509,7 +4580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2141147576"/>
+        <c:axId val="-2107694440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="12.0"/>
@@ -4521,7 +4592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2141144664"/>
+        <c:crossAx val="-2085273656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4696,11 +4767,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2142331736"/>
-        <c:axId val="2142674872"/>
+        <c:axId val="-2084487352"/>
+        <c:axId val="-2084507096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2142331736"/>
+        <c:axId val="-2084487352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4709,7 +4780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142674872"/>
+        <c:crossAx val="-2084507096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4717,7 +4788,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2142674872"/>
+        <c:axId val="-2084507096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4728,7 +4799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142331736"/>
+        <c:crossAx val="-2084487352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5689,11 +5760,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2144290136"/>
-        <c:axId val="-2144285032"/>
+        <c:axId val="-2084371960"/>
+        <c:axId val="-2083820648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2144290136"/>
+        <c:axId val="-2084371960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5702,7 +5773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144285032"/>
+        <c:crossAx val="-2083820648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5710,7 +5781,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144285032"/>
+        <c:axId val="-2083820648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10.0"/>
@@ -5722,7 +5793,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144290136"/>
+        <c:crossAx val="-2084371960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6677,11 +6748,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2144200584"/>
-        <c:axId val="-2144197448"/>
+        <c:axId val="-2083672616"/>
+        <c:axId val="-2083616984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2144200584"/>
+        <c:axId val="-2083672616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="-10.0"/>
@@ -6692,12 +6763,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144197448"/>
+        <c:crossAx val="-2083616984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2144197448"/>
+        <c:axId val="-2083616984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="18.0"/>
@@ -6709,7 +6780,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144200584"/>
+        <c:crossAx val="-2083672616"/>
         <c:crossesAt val="-17.0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7252,7 +7323,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7262,8 +7333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -9176,7 +9247,10 @@
         <f>AVERAGE(G3:G34)</f>
         <v>15.396864583333329</v>
       </c>
-      <c r="H36" s="1"/>
+      <c r="H36" s="1">
+        <f>AVERAGE(H3:H34)</f>
+        <v>14.625557911469631</v>
+      </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
         <f>AVERAGE(J3:J34)</f>
@@ -9190,7 +9264,10 @@
         <f>AVERAGE(L3:L34)</f>
         <v>-14.1232578125</v>
       </c>
-      <c r="M36" s="1"/>
+      <c r="M36" s="1">
+        <f>AVERAGE(M3:M34)</f>
+        <v>-12.554491281994759</v>
+      </c>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -9225,7 +9302,10 @@
         <f>_xlfn.STDEV.S(G3:G34)</f>
         <v>0.88145371072633505</v>
       </c>
-      <c r="H37" s="1"/>
+      <c r="H37" s="1">
+        <f>_xlfn.STDEV.S(H3:H34)</f>
+        <v>1.1046219019588832</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1">
         <f>_xlfn.STDEV.S(J3:J34)</f>
@@ -9239,7 +9319,10 @@
         <f>_xlfn.STDEV.S(L3:L34)</f>
         <v>0.63175009489249268</v>
       </c>
-      <c r="M37" s="1"/>
+      <c r="M37" s="1">
+        <f>_xlfn.STDEV.S(M3:M34)</f>
+        <v>0.48372721392903034</v>
+      </c>
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
       <c r="P37" s="9"/>
@@ -9272,16 +9355,42 @@
       <c r="AH37" s="13"/>
     </row>
     <row r="38" spans="2:34">
-      <c r="B38" s="10"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="B38" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="E38" s="1">
+        <f>MAX(E3:E34) - MIN(E3:E34)</f>
+        <v>4.277000000000001</v>
+      </c>
+      <c r="F38" s="1">
+        <f>MAX(F3:F34) - MIN(F3:F34)</f>
+        <v>3.5750000000000011</v>
+      </c>
+      <c r="G38" s="1">
+        <f>MAX(G3:G34) - MIN(G3:G34)</f>
+        <v>3.2740000000000009</v>
+      </c>
+      <c r="H38" s="1">
+        <f>MAX(H3:H34) - MIN(H3:H34)</f>
+        <v>4.2904433333333358</v>
+      </c>
       <c r="I38" s="8"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="J38" s="1">
+        <f>MAX(J3:J34) - MIN(J3:J34)</f>
+        <v>2.8599999999999994</v>
+      </c>
+      <c r="K38" s="1">
+        <f>MAX(K3:K34) - MIN(K3:K34)</f>
+        <v>2.5920000000000023</v>
+      </c>
+      <c r="L38" s="1">
+        <f>MAX(L3:L34) - MIN(L3:L34)</f>
+        <v>2.2699999999999996</v>
+      </c>
+      <c r="M38" s="1">
+        <f>MAX(M3:M34) - MIN(M3:M34)</f>
+        <v>1.8432500000000012</v>
+      </c>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
@@ -9328,6 +9437,8 @@
       <c r="B42" s="22"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
       <c r="M42" s="19"/>
       <c r="N42" s="30"/>
     </row>
@@ -9335,6 +9446,8 @@
       <c r="B43" s="17"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
       <c r="M43" s="19"/>
       <c r="N43" s="30"/>
     </row>
@@ -9342,6 +9455,8 @@
       <c r="B44" s="17"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
       <c r="M44" s="19"/>
       <c r="N44" s="30"/>
     </row>
@@ -9349,12 +9464,15 @@
       <c r="B45" s="17"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
       <c r="M45" s="19"/>
     </row>
     <row r="46" spans="2:34">
       <c r="B46" s="17"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
+      <c r="F46" s="8"/>
       <c r="M46" s="19"/>
       <c r="N46" s="30"/>
     </row>

</xml_diff>